<commit_message>
Changes related to vehicle renewal
</commit_message>
<xml_diff>
--- a/src/test/resources/TestDataFiles/VlsData.xlsx
+++ b/src/test/resources/TestDataFiles/VlsData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Work\IDrive-Sync\DevOps_Repos\vls-frontend-automation\src\test\resources\TestDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FE06CA-7447-4493-8EA7-3D34C18AC146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D451EB-AAFA-48AF-9D39-1EDBAD34718F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{3CFFB721-2F92-42A1-87DC-741A872FBFB8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27120" windowHeight="16590" activeTab="1" xr2:uid="{3CFFB721-2F92-42A1-87DC-741A872FBFB8}"/>
   </bookViews>
   <sheets>
     <sheet name="vehicleRenew" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="1221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="1222">
   <si>
     <t>ChassisNo</t>
   </si>
@@ -3593,81 +3593,21 @@
     <t>10981871</t>
   </si>
   <si>
-    <t>10108442</t>
-  </si>
-  <si>
-    <t>10037336</t>
-  </si>
-  <si>
-    <t>10227030</t>
-  </si>
-  <si>
-    <t>11059575</t>
-  </si>
-  <si>
-    <t>10110937</t>
-  </si>
-  <si>
-    <t>10028175</t>
-  </si>
-  <si>
-    <t>10242508</t>
-  </si>
-  <si>
     <t>10123916</t>
   </si>
   <si>
     <t>10175969</t>
   </si>
   <si>
-    <t>10095709</t>
-  </si>
-  <si>
-    <t>19XFB2642EE900908</t>
-  </si>
-  <si>
-    <t>19XFB2642FE900358</t>
-  </si>
-  <si>
-    <t>19XFB2643DE905114</t>
-  </si>
-  <si>
-    <t>19XFB2648DE903245</t>
-  </si>
-  <si>
-    <t>19XFB2677EE900574</t>
-  </si>
-  <si>
-    <t>19XFB2678DE905197</t>
-  </si>
-  <si>
-    <t>19XFC1690KE450058</t>
-  </si>
-  <si>
     <t>19XFC2670GE451996</t>
   </si>
   <si>
     <t>1B3CB2HA4AD654852</t>
   </si>
   <si>
-    <t>1C3AN69L34X003028</t>
-  </si>
-  <si>
-    <t>1C4AJWAG4GL244064</t>
-  </si>
-  <si>
     <t>1C4BJWAG3GL281207</t>
   </si>
   <si>
-    <t>1C4AJWAG6DL574395</t>
-  </si>
-  <si>
-    <t>1C4BJWAG0HL515319</t>
-  </si>
-  <si>
-    <t>1C4BJWAG5HL510830</t>
-  </si>
-  <si>
     <t>1C4BJWAG7EL135955</t>
   </si>
   <si>
@@ -3683,15 +3623,6 @@
     <t>10343518</t>
   </si>
   <si>
-    <t>10413516</t>
-  </si>
-  <si>
-    <t>11049136</t>
-  </si>
-  <si>
-    <t>10405469</t>
-  </si>
-  <si>
     <t>10107943</t>
   </si>
   <si>
@@ -3702,6 +3633,78 @@
   </si>
   <si>
     <t>10205926</t>
+  </si>
+  <si>
+    <t>1C4BJWAG7HL659675</t>
+  </si>
+  <si>
+    <t>1C4BJWAG9DL541721</t>
+  </si>
+  <si>
+    <t>1C4BJWAG9DL605076</t>
+  </si>
+  <si>
+    <t>1C4BJWBG1GL123978</t>
+  </si>
+  <si>
+    <t>1C4BJWBG5CL140020</t>
+  </si>
+  <si>
+    <t>1C4BJWBG8FL540982</t>
+  </si>
+  <si>
+    <t>1C4BJWBGXEL230315</t>
+  </si>
+  <si>
+    <t>1C4BJWDG5EL153155</t>
+  </si>
+  <si>
+    <t>1C4BJWDG6GL149036</t>
+  </si>
+  <si>
+    <t>1C4BJWDG9JL801655</t>
+  </si>
+  <si>
+    <t>1C4BJWDGXFL734555</t>
+  </si>
+  <si>
+    <t>1C4BJWEG2FL582057</t>
+  </si>
+  <si>
+    <t>10343825</t>
+  </si>
+  <si>
+    <t>10238585</t>
+  </si>
+  <si>
+    <t>10228361</t>
+  </si>
+  <si>
+    <t>10144267</t>
+  </si>
+  <si>
+    <t>10455470</t>
+  </si>
+  <si>
+    <t>10268377</t>
+  </si>
+  <si>
+    <t>10527296</t>
+  </si>
+  <si>
+    <t>10254224</t>
+  </si>
+  <si>
+    <t>10152681</t>
+  </si>
+  <si>
+    <t>10242915</t>
+  </si>
+  <si>
+    <t>10249326</t>
+  </si>
+  <si>
+    <t>10043482</t>
   </si>
 </sst>
 </file>
@@ -3784,6 +3787,26 @@
   <dxfs count="22">
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -3860,16 +3883,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
@@ -3956,16 +3969,6 @@
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -3984,10 +3987,10 @@
   <autoFilter ref="A1:I28" xr:uid="{BA43C8AF-8592-4BDE-B541-FBCD2E9E2A04}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D5ABAE62-F064-4479-8A0F-39CE4CD9BE17}" name="ChassisNo"/>
-    <tableColumn id="2" xr3:uid="{7AE215EB-3C0F-49F7-BD57-A0939740306F}" name="RTAUnifiedNo" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{9EAA0457-8746-4CEA-BC9C-9142AA53FB77}" name="EID" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{2AAFDEC5-A3A6-41EC-B2EC-83AA19425BC8}" name="Expiry Date" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{3D0AC05E-9757-4591-9AA3-20F36A5A4BBA}" name="Scenario" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{7AE215EB-3C0F-49F7-BD57-A0939740306F}" name="RTAUnifiedNo" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{9EAA0457-8746-4CEA-BC9C-9142AA53FB77}" name="EID" dataDxfId="20"/>
+    <tableColumn id="4" xr3:uid="{2AAFDEC5-A3A6-41EC-B2EC-83AA19425BC8}" name="Expiry Date" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{3D0AC05E-9757-4591-9AA3-20F36A5A4BBA}" name="Scenario" dataDxfId="18"/>
     <tableColumn id="6" xr3:uid="{B9CEDD55-8E92-4733-8C88-A152FBA5975B}" name="Comments"/>
     <tableColumn id="7" xr3:uid="{DDA849C1-9D4A-40EE-B133-80B15E500A58}" name="PLATE"/>
     <tableColumn id="8" xr3:uid="{6B3BCED6-2029-422E-B4DE-CE73643844B7}" name="CODE"/>
@@ -3998,12 +4001,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{57C5D3D0-5773-F348-BF21-DF63A5E2D37D}" name="Table4" displayName="Table4" ref="A1:C518" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:C518" xr:uid="{57C5D3D0-5773-F348-BF21-DF63A5E2D37D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{57C5D3D0-5773-F348-BF21-DF63A5E2D37D}" name="Table4" displayName="Table4" ref="A1:C508" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:C508" xr:uid="{57C5D3D0-5773-F348-BF21-DF63A5E2D37D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{636F7DCD-107C-B644-9664-A25980CFF7B8}" name="RTAUnifiedNo" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{767B43EC-3BAF-3C4B-B2C5-CFC666484FE5}" name="Chassis No" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{6089DB15-9ABB-8B42-A4E8-3F2228C6774A}" name="Column1" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{636F7DCD-107C-B644-9664-A25980CFF7B8}" name="RTAUnifiedNo" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{767B43EC-3BAF-3C4B-B2C5-CFC666484FE5}" name="Chassis No" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{6089DB15-9ABB-8B42-A4E8-3F2228C6774A}" name="Column1" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4015,8 +4018,8 @@
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{988E83EA-0391-494B-A4DA-E73CEC3E81F9}" name="CHASSIS_NO"/>
     <tableColumn id="2" xr3:uid="{2AB8AD22-6B6A-495E-A85C-2EAE0767F2E5}" name="RTA_UNIFIED_NO"/>
-    <tableColumn id="3" xr3:uid="{42F314F2-5A70-43ED-B17F-B1E3645F087C}" name="EID_NUMBER" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{EF8FE431-ED2F-496D-A849-5DD701815414}" name="EXPIRY_DATE" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{42F314F2-5A70-43ED-B17F-B1E3645F087C}" name="EID_NUMBER" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{EF8FE431-ED2F-496D-A849-5DD701815414}" name="EXPIRY_DATE" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{236CB861-D01B-4536-8F9D-CB5828495AAA}" name="PLATE"/>
     <tableColumn id="6" xr3:uid="{7DC6B2D3-3B64-48E1-82B5-94CFD818961C}" name="CODE"/>
     <tableColumn id="7" xr3:uid="{EEC6FDCF-243B-473A-9DE6-319BABFB5FBE}" name="RTA_ID"/>
@@ -4031,10 +4034,10 @@
   <autoFilter ref="A1:F28" xr:uid="{BA43C8AF-8592-4BDE-B541-FBCD2E9E2A04}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{09F9DACB-7CDE-4ACD-9806-1B3C6F92AD1D}" name="ChassisNo"/>
-    <tableColumn id="2" xr3:uid="{9D504645-242C-425E-B492-4E7F8E26E220}" name="RTAUnifiedNo" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{41CBA1D6-E204-4965-9504-2998A3DF423B}" name="EID" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{05E15DD4-3AD0-434B-B053-494FB65D3BB8}" name="Expiry Date" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{D8D7E5C7-426A-41DE-8AA0-A69A7ACA152D}" name="Scenario" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{9D504645-242C-425E-B492-4E7F8E26E220}" name="RTAUnifiedNo" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{41CBA1D6-E204-4965-9504-2998A3DF423B}" name="EID" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{05E15DD4-3AD0-434B-B053-494FB65D3BB8}" name="Expiry Date" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{D8D7E5C7-426A-41DE-8AA0-A69A7ACA152D}" name="Scenario" dataDxfId="7"/>
     <tableColumn id="6" xr3:uid="{79822E8C-C523-467F-BF59-D93076FB98AE}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -4042,12 +4045,12 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D0C053EB-00CA-4008-983B-00854B233396}" name="Table46" displayName="Table46" ref="A1:C527" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D0C053EB-00CA-4008-983B-00854B233396}" name="Table46" displayName="Table46" ref="A1:C527" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:C527" xr:uid="{57C5D3D0-5773-F348-BF21-DF63A5E2D37D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4D55C113-B045-4846-B010-91B19377D03D}" name="RTAUnifiedNo" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{8B521B43-4C28-40F2-A86A-65E40EAF00E1}" name="Chassis No" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{41625F0B-3BE1-4E51-9C6D-F8084EE33DB2}" name="Column1" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{4D55C113-B045-4846-B010-91B19377D03D}" name="RTAUnifiedNo" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{8B521B43-4C28-40F2-A86A-65E40EAF00E1}" name="Chassis No" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{41625F0B-3BE1-4E51-9C6D-F8084EE33DB2}" name="Column1" dataDxfId="2">
       <calculatedColumnFormula>TEXT(Table46[[#This Row],[RTAUnifiedNo]],Table46[[#This Row],[RTAUnifiedNo]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4818,7 +4821,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:A1048576 A1:A18">
-    <cfRule type="duplicateValues" dxfId="21" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -4830,7 +4833,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB1D62C-99C7-7B47-A4E2-CBE198EE5193}">
-  <dimension ref="A1:C518"/>
+  <dimension ref="A1:C508"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A20"/>
@@ -4859,7 +4862,7 @@
         <v>1184</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>1194</v>
+        <v>1186</v>
       </c>
       <c r="C2" s="12"/>
     </row>
@@ -4868,106 +4871,106 @@
         <v>1185</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>1195</v>
+        <v>1187</v>
       </c>
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" ht="21">
       <c r="A4" s="11" t="s">
-        <v>1186</v>
+        <v>1193</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>1196</v>
+        <v>1188</v>
       </c>
       <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" ht="21">
       <c r="A5" s="11" t="s">
-        <v>1187</v>
+        <v>1195</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>1197</v>
+        <v>1190</v>
       </c>
       <c r="C5" s="12"/>
     </row>
     <row r="6" spans="1:3" ht="21">
       <c r="A6" s="11" t="s">
-        <v>1188</v>
+        <v>1196</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>1198</v>
+        <v>1191</v>
       </c>
       <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" ht="21">
       <c r="A7" s="11" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>1189</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>1199</v>
       </c>
       <c r="C7" s="12"/>
     </row>
     <row r="8" spans="1:3" ht="21">
       <c r="A8" s="11" t="s">
-        <v>1190</v>
+        <v>1197</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>1200</v>
+        <v>1192</v>
       </c>
       <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3" ht="21">
       <c r="A9" s="11" t="s">
-        <v>1191</v>
+        <v>1214</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>1201</v>
+        <v>1202</v>
       </c>
       <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:3" ht="21">
       <c r="A10" s="11" t="s">
-        <v>1192</v>
+        <v>1210</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>1202</v>
+        <v>1198</v>
       </c>
       <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:3" ht="21">
       <c r="A11" s="11" t="s">
-        <v>1193</v>
+        <v>1211</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>1203</v>
+        <v>1199</v>
       </c>
       <c r="C11" s="12"/>
     </row>
     <row r="12" spans="1:3" ht="21">
       <c r="A12" s="11" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>1205</v>
+        <v>1200</v>
       </c>
       <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3" ht="21">
       <c r="A13" s="11" t="s">
-        <v>670</v>
+        <v>1213</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
       <c r="C13" s="12"/>
     </row>
     <row r="14" spans="1:3" ht="21">
       <c r="A14" s="11" t="s">
-        <v>1214</v>
+        <v>1216</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>1206</v>
+        <v>1204</v>
       </c>
       <c r="C14" s="12"/>
     </row>
@@ -4976,16 +4979,16 @@
         <v>1215</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>1207</v>
+        <v>1203</v>
       </c>
       <c r="C15" s="12"/>
     </row>
     <row r="16" spans="1:3" ht="21">
       <c r="A16" s="11" t="s">
-        <v>1216</v>
+        <v>1218</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>1208</v>
+        <v>1206</v>
       </c>
       <c r="C16" s="12"/>
     </row>
@@ -4994,34 +4997,34 @@
         <v>1217</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>1209</v>
+        <v>1205</v>
       </c>
       <c r="C17" s="12"/>
     </row>
     <row r="18" spans="1:3" ht="21">
       <c r="A18" s="11" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" ht="21">
       <c r="A19" s="11" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="C19" s="12"/>
     </row>
     <row r="20" spans="1:3" ht="21">
       <c r="A20" s="11" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="C20" s="12"/>
     </row>
@@ -7464,56 +7467,6 @@
       <c r="A508" s="11"/>
       <c r="B508" s="10"/>
       <c r="C508" s="10"/>
-    </row>
-    <row r="509" spans="1:3" ht="21">
-      <c r="A509" s="11"/>
-      <c r="B509" s="10"/>
-      <c r="C509" s="10"/>
-    </row>
-    <row r="510" spans="1:3" ht="21">
-      <c r="A510" s="11"/>
-      <c r="B510" s="10"/>
-      <c r="C510" s="10"/>
-    </row>
-    <row r="511" spans="1:3" ht="21">
-      <c r="A511" s="11"/>
-      <c r="B511" s="10"/>
-      <c r="C511" s="10"/>
-    </row>
-    <row r="512" spans="1:3" ht="21">
-      <c r="A512" s="11"/>
-      <c r="B512" s="10"/>
-      <c r="C512" s="10"/>
-    </row>
-    <row r="513" spans="1:3" ht="21">
-      <c r="A513" s="11"/>
-      <c r="B513" s="10"/>
-      <c r="C513" s="10"/>
-    </row>
-    <row r="514" spans="1:3" ht="21">
-      <c r="A514" s="11"/>
-      <c r="B514" s="10"/>
-      <c r="C514" s="10"/>
-    </row>
-    <row r="515" spans="1:3" ht="21">
-      <c r="A515" s="11"/>
-      <c r="B515" s="10"/>
-      <c r="C515" s="10"/>
-    </row>
-    <row r="516" spans="1:3" ht="21">
-      <c r="A516" s="11"/>
-      <c r="B516" s="10"/>
-      <c r="C516" s="10"/>
-    </row>
-    <row r="517" spans="1:3" ht="21">
-      <c r="A517" s="11"/>
-      <c r="B517" s="10"/>
-      <c r="C517" s="10"/>
-    </row>
-    <row r="518" spans="1:3" ht="21">
-      <c r="A518" s="11"/>
-      <c r="B518" s="10"/>
-      <c r="C518" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -8777,7 +8730,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>